<commit_message>
finally got working report generator
</commit_message>
<xml_diff>
--- a/public/exports/blank-template.xlsx
+++ b/public/exports/blank-template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>LAPORAN DATA SEMUA TADIKA YANG ADA BAGI TAHUN 2022.</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>NAMA KP YANG TERLIBAT</t>
-  </si>
-  <si>
-    <t>Report Generated by Gi-Ret 2.0 on 27/02/2022 at 14:47</t>
   </si>
 </sst>
 </file>
@@ -386,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -422,11 +419,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>